<commit_message>
adicionando codigo do EP2
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\AED2\EP1\EP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B691110-970C-4796-AAED-46DF003163B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89822FBF-97D3-4734-9F21-472A9D0EF54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8B41032B-D40C-4622-97EE-8103E51893AB}"/>
   </bookViews>
@@ -17,25 +17,10 @@
     <sheet name="Planilha4" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Planilha9!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Planilha9!$A$2:$A$114</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Planilha9!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Planilha9!$B$2:$B$114</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Planilha9!$A$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Planilha9!$A$2:$A$114</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Planilha9!$B$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Planilha9!$B$2:$B$114</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Planilha9!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Planilha9!$B$2:$B$114</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Planilha9!$A$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Planilha9!$A$2:$A$114</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Planilha9!$B$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Planilha9!$B$2:$B$114</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Planilha9!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Planilha9!$A$2:$A$114</definedName>
     <definedName name="DadosExternos_1" localSheetId="0" hidden="1">Planilha9!$A$1:$B$114</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>